<commit_message>
Parsing schema with refs, temporary progress
--HG--
branch : EPBDS-9746
</commit_message>
<xml_diff>
--- a/Util/openl-openapi-model-scaffolding/resources/datatype_template.xlsx
+++ b/Util/openl-openapi-model-scaffolding/resources/datatype_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Util\openl-openapi-model-scaffolding\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CDCBF4-6EDC-4078-89D9-87E741B11CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540675D1-073D-4E1E-B6D2-9CFE050A0C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="6450" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0AEC756-2EC7-4462-B805-D4D599FFC0B7}"/>
   </bookViews>
@@ -60,8 +60,14 @@
     <t>Value</t>
   </si>
   <si>
+    <t>{spr.step.name}</t>
+  </si>
+  <si>
+    <t>{spr.step.value}</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
+      <t xml:space="preserve">Spreadsheet {spr.return.type} </t>
     </r>
     <r>
       <rPr>
@@ -73,12 +79,6 @@
       </rPr>
       <t>{spr.name.template}</t>
     </r>
-  </si>
-  <si>
-    <t>{spr.step.name}</t>
-  </si>
-  <si>
-    <t>{spr.step.value}</t>
   </si>
 </sst>
 </file>
@@ -414,6 +414,9 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -436,9 +439,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -767,11 +767,11 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
@@ -797,7 +797,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -808,11 +808,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.85">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="15.3" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A2" s="4" t="s">
@@ -824,21 +824,21 @@
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="17.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.65">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>